<commit_message>
Changed Rubic Add Comment to credit Dan
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -968,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="H4" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1129,11 +1129,15 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1238,7 +1242,7 @@
       </c>
       <c r="H8" s="19">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -2467,11 +2471,15 @@
       <c r="D65" s="5">
         <v>1</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
+      <c r="E65" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G65" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -2492,11 +2500,15 @@
       <c r="D66" s="5">
         <v>1</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G66" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -3083,7 +3095,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added DirLight Added Point Light Have both lights moving
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -74,12 +74,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="A73" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -968,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1112,7 @@
       </c>
       <c r="H4" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1109,11 +1124,11 @@
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1166,15 +1181,19 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 18,0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I6" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 18,0)</f>
@@ -1242,11 +1261,11 @@
       </c>
       <c r="H8" s="19">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I8" s="18">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1307,7 +1326,7 @@
       </c>
       <c r="H10" s="20">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -1464,11 +1483,15 @@
       <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1726,11 +1749,15 @@
       <c r="D30" s="5">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G30" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1751,11 +1778,15 @@
       <c r="D31" s="5">
         <v>2</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G31" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1801,11 +1832,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G33" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1826,11 +1861,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G34" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1851,11 +1890,15 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G35" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2300,11 +2343,15 @@
       <c r="D56" s="5">
         <v>3</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G56" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>

</xml_diff>

<commit_message>
Fixed Lighting Changed Excel
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,79 @@
             <family val="2"/>
           </rPr>
           <t>The full web address from GitHub.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+WHITE COLOR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PURPLE COLOR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Look at the pyramid in the scene to see the lights move
+</t>
         </r>
       </text>
     </comment>
@@ -983,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3215,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Spot Light Added Sky Box Cleaned Up Some Code Changed plane
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>Student Name: Timothy Felice | tmfelice@fullsail.edu</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1187,7 +1192,7 @@
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1195,11 +1200,11 @@
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1252,19 +1257,15 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 18,0)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I6" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 18,0)</f>
@@ -1340,7 +1341,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1397,11 +1398,11 @@
       </c>
       <c r="H10" s="20">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -1683,11 +1684,15 @@
       <c r="D23" s="5">
         <v>3</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1878,11 +1883,15 @@
       <c r="D32" s="5">
         <v>2</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1990,11 +1999,15 @@
       <c r="D36" s="5">
         <v>1</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="17">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -3059,7 +3072,9 @@
       <c r="C90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -3079,7 +3094,9 @@
       <c r="C91" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3213,7 +3230,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Finished View Port And Did instancing Commit for Milestone 2
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="I4" s="18">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1257,11 +1257,15 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="18">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 18, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 18,0)</f>
@@ -1341,7 +1345,7 @@
       </c>
       <c r="J8" s="18">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1402,7 +1406,7 @@
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -2660,11 +2664,15 @@
       <c r="D67" s="5">
         <v>4</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G67" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -3230,7 +3238,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Worked On Normal Mapping Changed Asset Folder
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -95,6 +95,31 @@
           </rPr>
           <t xml:space="preserve">
 PURPLE COLOR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Blue Light
+</t>
         </r>
       </text>
     </comment>
@@ -1059,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Got Spectacular Mapping Working
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1310,7 +1310,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="16">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1695,11 +1695,15 @@
       <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -2114,11 +2118,15 @@
       <c r="D39" s="5">
         <v>2</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -3274,7 +3282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added Spec to rubric
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1310,7 +1310,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="16">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2147,11 +2147,15 @@
       <c r="D40" s="5">
         <v>2</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G40" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3282,7 +3286,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Got Geo Instancing Done
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1310,7 +1310,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="16">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1395,11 +1395,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G9" s="17">
         <f xml:space="preserve"> IF(EXACT(F9,"X"),IF(EXACT(E9,"I"),$B9,IF(EXACT(E9,"II"),$C9,IF(EXACT(E9,"III"),$D9,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="20" t="s">
         <v>26</v>
@@ -1442,7 +1446,7 @@
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>

</xml_diff>

<commit_message>
Final Turn In Commit
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,15 +1224,15 @@
       </c>
       <c r="J4" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="K4" s="18">
         <f>SUM(H6,I6,J6)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L4" s="18">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1305,12 +1305,12 @@
       </c>
       <c r="J6" s="18">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 18, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 18,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="16">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1438,15 +1438,15 @@
       </c>
       <c r="H10" s="20">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I10" s="20">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J10" s="20">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1649,11 +1649,15 @@
       <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2454,11 +2458,15 @@
       <c r="D55" s="5">
         <v>2</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2870,11 +2878,15 @@
       <c r="D75" s="5">
         <v>4</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G75" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -3290,7 +3302,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>